<commit_message>
Adding test method, where test data taken from XLSX file.
</commit_message>
<xml_diff>
--- a/Luma/tests/Test07_ReadFromFileAndSearch.xlsx
+++ b/Luma/tests/Test07_ReadFromFileAndSearch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git-project\luma-repo\Luma\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556946EE-E6FD-43E3-B8BD-C18C2AFDF4E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDEF1F5-ABB7-4C74-9BAE-994CBECAA12F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31935" yWindow="8235" windowWidth="21120" windowHeight="9705" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30300" yWindow="3165" windowWidth="21120" windowHeight="9705" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchResults" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>data_id</t>
   </si>
@@ -52,13 +52,25 @@
     <t>search_2</t>
   </si>
   <si>
-    <t>tank</t>
-  </si>
-  <si>
     <t>read_1</t>
   </si>
   <si>
     <t>Man</t>
+  </si>
+  <si>
+    <t>search_3</t>
+  </si>
+  <si>
+    <t>search_4</t>
+  </si>
+  <si>
+    <t>pants</t>
+  </si>
+  <si>
+    <t>TAURUS</t>
+  </si>
+  <si>
+    <t>Backpack</t>
   </si>
 </sst>
 </file>
@@ -382,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,7 +434,32 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -459,10 +496,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
       </c>
       <c r="C2">
         <v>12</v>

</xml_diff>

<commit_message>
Refactoring results_page.py and adding page locators.
</commit_message>
<xml_diff>
--- a/Luma/tests/Test07_ReadFromFileAndSearch.xlsx
+++ b/Luma/tests/Test07_ReadFromFileAndSearch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git-project\luma-repo\Luma\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDEF1F5-ABB7-4C74-9BAE-994CBECAA12F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036D1330-04C6-4281-94EA-C778D9CAE653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30300" yWindow="3165" windowWidth="21120" windowHeight="9705" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4005" yWindow="2940" windowWidth="21120" windowHeight="9705" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchResults" sheetId="1" r:id="rId1"/>
@@ -397,7 +397,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>